<commit_message>
Developpement de solve et bugfix
</commit_message>
<xml_diff>
--- a/Tests.xlsx
+++ b/Tests.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laurent\Documents\Uni\SessionHiver2022\SIAD\ProjetSession\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laure\Documents\Université\Session 4\SIAD\TP2_SIAD_equipe7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8835244A-EDD2-4A63-95D9-DA605A28F0EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C3ACCE-B86F-40DA-80D7-79FE66DD689B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Temps" sheetId="1" r:id="rId1"/>
@@ -678,7 +678,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,7 +702,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>50</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -713,7 +713,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -724,7 +724,7 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>20</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fonctionnel sans check du Excel ou de la solution
</commit_message>
<xml_diff>
--- a/Tests.xlsx
+++ b/Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laurent\Documents\Uni\SessionHiver2022\SIAD\TP2_SIAD_equipe7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CDA9CA7-15C6-49A2-9B47-5AACF906C4B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CBAA870-6750-4B7E-AABB-CE5FDA625F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16080" yWindow="1560" windowWidth="12600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="16080" yWindow="1560" windowWidth="12600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Temps" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="19">
   <si>
     <t>A</t>
   </si>
@@ -77,6 +77,12 @@
   </si>
   <si>
     <t>Type</t>
+  </si>
+  <si>
+    <t>Cout d'usage</t>
+  </si>
+  <si>
+    <t>Cout fixe</t>
   </si>
 </sst>
 </file>
@@ -394,15 +400,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F2:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -412,11 +418,11 @@
       <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -426,11 +432,11 @@
       <c r="C2">
         <v>5.8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -440,11 +446,11 @@
       <c r="C3">
         <v>14.3</v>
       </c>
-      <c r="E3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -454,11 +460,11 @@
       <c r="C4">
         <v>16.600000000000001</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -468,11 +474,11 @@
       <c r="C5">
         <v>19.600000000000001</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -482,11 +488,11 @@
       <c r="C6">
         <v>18.100000000000001</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -496,11 +502,11 @@
       <c r="C7">
         <v>54.8</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -510,11 +516,11 @@
       <c r="C8">
         <v>19.8</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -525,7 +531,7 @@
         <v>19.5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -536,7 +542,7 @@
         <v>25.1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -547,7 +553,7 @@
         <v>13.7</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -558,7 +564,7 @@
         <v>60.3</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -569,7 +575,7 @@
         <v>24.3</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -580,7 +586,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -591,7 +597,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -675,15 +681,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B5B958-4166-4E45-A9D7-085E479A7EAF}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -693,8 +699,14 @@
       <c r="C1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -704,8 +716,14 @@
       <c r="C2">
         <v>120</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -715,8 +733,14 @@
       <c r="C3">
         <v>90</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -725,6 +749,12 @@
       </c>
       <c r="C4">
         <v>65</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Preparation pour implémentation des jours
</commit_message>
<xml_diff>
--- a/Tests.xlsx
+++ b/Tests.xlsx
@@ -8,25 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laurent\Documents\Uni\SessionHiver2022\SIAD\TP2_SIAD_equipe7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CBAA870-6750-4B7E-AABB-CE5FDA625F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB0EC39-9530-42D6-9C86-7FE39EEE50FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="16080" yWindow="1560" windowWidth="12600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Temps" sheetId="1" r:id="rId1"/>
     <sheet name="Camions" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="20">
   <si>
     <t>A</t>
   </si>
@@ -83,6 +93,9 @@
   </si>
   <si>
     <t>Cout fixe</t>
+  </si>
+  <si>
+    <t>Temps_total</t>
   </si>
 </sst>
 </file>
@@ -400,15 +413,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F2:F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -421,8 +434,11 @@
       <c r="F1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -435,8 +451,11 @@
       <c r="F2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -449,8 +468,11 @@
       <c r="F3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -463,8 +485,11 @@
       <c r="F4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -477,8 +502,11 @@
       <c r="F5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -491,8 +519,11 @@
       <c r="F6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -505,8 +536,11 @@
       <c r="F7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -519,8 +553,11 @@
       <c r="F8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -531,7 +568,7 @@
         <v>19.5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -542,7 +579,7 @@
         <v>25.1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -553,7 +590,7 @@
         <v>13.7</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -564,7 +601,7 @@
         <v>60.3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -575,7 +612,7 @@
         <v>24.3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -586,7 +623,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -597,7 +634,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -683,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B5B958-4166-4E45-A9D7-085E479A7EAF}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,7 +751,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D2">
         <v>5</v>
@@ -731,7 +768,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -748,7 +785,7 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>65</v>
+        <v>20</v>
       </c>
       <c r="D4">
         <v>3</v>

</xml_diff>